<commit_message>
Refactor agreement calculation methods and update thresholds; remove unused weighted voting logic
</commit_message>
<xml_diff>
--- a/results/agreement_metrics/feature_human_agreement.xlsx
+++ b/results/agreement_metrics/feature_human_agreement.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="24360" windowHeight="14145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -107,16 +107,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="178" formatCode="0.0%"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -124,7 +128,7 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -132,11 +136,162 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +310,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -179,23 +520,317 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -478,46 +1113,53 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.375" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="5.875" customWidth="1"/>
+    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="7" max="7" width="15.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>-0.09006928406466508</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-0.0900692840646651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -525,7 +1167,7 @@
         <v>0.3375</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -533,7 +1175,7 @@
         <v>0.8375</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -541,7 +1183,7 @@
         <v>0.8875</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -549,7 +1191,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -579,7 +1221,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="4">
-        <v>-0.09006928406466508</v>
+        <v>-0.0900692840646651</v>
       </c>
       <c r="C13" s="5">
         <v>0.3375</v>
@@ -594,17 +1236,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -612,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -620,7 +1262,7 @@
         <v>0.3875</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -628,7 +1270,7 @@
         <v>0.8375</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -636,7 +1278,7 @@
         <v>1.1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -644,7 +1286,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -689,25 +1331,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:1">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="4">
-        <v>-0.02468560782487206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>-0.0246856078248721</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -715,7 +1357,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
@@ -723,7 +1365,7 @@
         <v>0.8375</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
@@ -731,7 +1373,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -739,7 +1381,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -769,7 +1411,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="4">
-        <v>-0.02468560782487206</v>
+        <v>-0.0246856078248721</v>
       </c>
       <c r="C39" s="5">
         <v>0.375</v>
@@ -784,25 +1426,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:1">
       <c r="A42" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:1">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:2">
       <c r="A44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="4">
-        <v>-0.05839416058394176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-0.0583941605839418</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="3" t="s">
         <v>4</v>
       </c>
@@ -810,7 +1452,7 @@
         <v>0.425</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:2">
       <c r="A46" s="3" t="s">
         <v>5</v>
       </c>
@@ -818,7 +1460,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:2">
       <c r="A47" s="3" t="s">
         <v>6</v>
       </c>
@@ -826,7 +1468,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -834,7 +1476,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:1">
       <c r="A50" s="2" t="s">
         <v>8</v>
       </c>
@@ -864,7 +1506,7 @@
         <v>18</v>
       </c>
       <c r="B52" s="4">
-        <v>-0.05839416058394176</v>
+        <v>-0.0583941605839418</v>
       </c>
       <c r="C52" s="5">
         <v>0.425</v>
@@ -879,17 +1521,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:1">
       <c r="A55" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:1">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:2">
       <c r="A57" s="3" t="s">
         <v>3</v>
       </c>
@@ -897,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:2">
       <c r="A58" s="3" t="s">
         <v>4</v>
       </c>
@@ -905,7 +1547,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:2">
       <c r="A59" s="3" t="s">
         <v>5</v>
       </c>
@@ -913,7 +1555,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:2">
       <c r="A60" s="3" t="s">
         <v>6</v>
       </c>
@@ -921,7 +1563,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
@@ -929,7 +1571,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:1">
       <c r="A63" s="2" t="s">
         <v>8</v>
       </c>
@@ -974,25 +1616,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:1">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:1">
       <c r="A69" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="4">
-        <v>0.02877697841726612</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>0.0287769784172661</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1642,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
         <v>5</v>
       </c>
@@ -1008,7 +1650,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1658,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1666,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:1">
       <c r="A76" s="2" t="s">
         <v>8</v>
       </c>
@@ -1054,7 +1696,7 @@
         <v>18</v>
       </c>
       <c r="B78" s="4">
-        <v>0.02877697841726612</v>
+        <v>0.0287769784172661</v>
       </c>
       <c r="C78" s="5">
         <v>0.45</v>
@@ -1069,17 +1711,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:1">
       <c r="A81" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:1">
       <c r="A82" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1729,7 @@
         <v>0.107736117702895</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1737,7 @@
         <v>0.475</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
         <v>5</v>
       </c>
@@ -1103,7 +1745,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
         <v>6</v>
       </c>
@@ -1111,7 +1753,7 @@
         <v>0.7375</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
         <v>7</v>
       </c>
@@ -1119,7 +1761,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:1">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
@@ -1164,17 +1806,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:1">
       <c r="A94" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:1">
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:2">
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
@@ -1182,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:2">
       <c r="A97" s="3" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1832,7 @@
         <v>0.5125</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:2">
       <c r="A98" s="3" t="s">
         <v>5</v>
       </c>
@@ -1198,7 +1840,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:2">
       <c r="A99" s="3" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:2">
       <c r="A100" s="3" t="s">
         <v>7</v>
       </c>
@@ -1214,7 +1856,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:1">
       <c r="A102" s="2" t="s">
         <v>8</v>
       </c>
@@ -1259,25 +1901,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:1">
       <c r="A107" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:1">
       <c r="A108" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:2">
       <c r="A109" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B109" s="4">
-        <v>0.1102697586370091</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+        <v>0.110269758637009</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
       <c r="A110" s="3" t="s">
         <v>4</v>
       </c>
@@ -1285,7 +1927,7 @@
         <v>0.475</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:2">
       <c r="A111" s="3" t="s">
         <v>5</v>
       </c>
@@ -1293,7 +1935,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:2">
       <c r="A112" s="3" t="s">
         <v>6</v>
       </c>
@@ -1301,7 +1943,7 @@
         <v>0.7375</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:2">
       <c r="A113" s="3" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1951,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:1">
       <c r="A115" s="2" t="s">
         <v>8</v>
       </c>
@@ -1339,7 +1981,7 @@
         <v>22</v>
       </c>
       <c r="B117" s="4">
-        <v>0.1102697586370091</v>
+        <v>0.110269758637009</v>
       </c>
       <c r="C117" s="5">
         <v>0.475</v>
@@ -1354,25 +1996,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:1">
       <c r="A120" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:1">
       <c r="A121" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:2">
       <c r="A122" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B122" s="4">
-        <v>-0.05121293800539095</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+        <v>-0.051212938005391</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
       <c r="A123" s="3" t="s">
         <v>4</v>
       </c>
@@ -1380,7 +2022,7 @@
         <v>0.525</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:2">
       <c r="A124" s="3" t="s">
         <v>5</v>
       </c>
@@ -1388,7 +2030,7 @@
         <v>0.975</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:2">
       <c r="A125" s="3" t="s">
         <v>6</v>
       </c>
@@ -1396,7 +2038,7 @@
         <v>0.5125</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:2">
       <c r="A126" s="3" t="s">
         <v>7</v>
       </c>
@@ -1404,7 +2046,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:1">
       <c r="A128" s="2" t="s">
         <v>8</v>
       </c>
@@ -1434,7 +2076,7 @@
         <v>26</v>
       </c>
       <c r="B130" s="4">
-        <v>-0.05121293800539095</v>
+        <v>-0.051212938005391</v>
       </c>
       <c r="C130" s="5">
         <v>0.525</v>
@@ -1449,17 +2091,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:1">
       <c r="A133" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:1">
       <c r="A134" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:2">
       <c r="A135" s="3" t="s">
         <v>3</v>
       </c>
@@ -1467,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:2">
       <c r="A136" s="3" t="s">
         <v>4</v>
       </c>
@@ -1475,7 +2117,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:2">
       <c r="A137" s="3" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +2125,7 @@
         <v>0.975</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:2">
       <c r="A138" s="3" t="s">
         <v>6</v>
       </c>
@@ -1491,7 +2133,7 @@
         <v>0.225</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:2">
       <c r="A139" s="3" t="s">
         <v>7</v>
       </c>
@@ -1499,7 +2141,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:1">
       <c r="A141" s="2" t="s">
         <v>8</v>
       </c>
@@ -1544,17 +2186,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:1">
       <c r="A146" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:1">
       <c r="A147" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:2">
       <c r="A148" s="3" t="s">
         <v>3</v>
       </c>
@@ -1562,7 +2204,7 @@
         <v>-0.0714285714285714</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:2">
       <c r="A149" s="3" t="s">
         <v>4</v>
       </c>
@@ -1570,7 +2212,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:2">
       <c r="A150" s="3" t="s">
         <v>5</v>
       </c>
@@ -1578,7 +2220,7 @@
         <v>0.975</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:2">
       <c r="A151" s="3" t="s">
         <v>6</v>
       </c>
@@ -1586,7 +2228,7 @@
         <v>0.475</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:2">
       <c r="A152" s="3" t="s">
         <v>7</v>
       </c>
@@ -1594,7 +2236,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:1">
       <c r="A154" s="2" t="s">
         <v>8</v>
       </c>
@@ -1641,5 +2283,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: completely removed pron-complexity
</commit_message>
<xml_diff>
--- a/results/agreement_metrics/feature_human_agreement.xlsx
+++ b/results/agreement_metrics/feature_human_agreement.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="24360" windowHeight="14145"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -107,20 +107,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
-    <numFmt numFmtId="178" formatCode="0.0%"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -128,7 +124,7 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -136,162 +132,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,194 +155,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -520,317 +179,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1113,61 +478,54 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.375" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
-    <col min="4" max="4" width="15.375" customWidth="1"/>
-    <col min="5" max="5" width="5.875" customWidth="1"/>
-    <col min="6" max="6" width="5.625" customWidth="1"/>
-    <col min="7" max="7" width="15.7083333333333" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>-0.0900692840646651</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>0.2830188679245284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5">
-        <v>0.3375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>0.5375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1175,15 +533,15 @@
         <v>0.8375</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>0.8875</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +549,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1221,64 +579,64 @@
         <v>14</v>
       </c>
       <c r="B13" s="4">
-        <v>-0.0900692840646651</v>
+        <v>0.2830188679245284</v>
       </c>
       <c r="C13" s="5">
-        <v>0.3375</v>
+        <v>0.5375</v>
       </c>
       <c r="D13" s="5">
         <v>0.8375</v>
       </c>
       <c r="E13" s="4">
-        <v>0.8875</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>0.2103639728562615</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="5">
-        <v>0.3875</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="5">
-        <v>0.8375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="4">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +644,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1316,40 +674,40 @@
         <v>14</v>
       </c>
       <c r="B26" s="4">
-        <v>0</v>
+        <v>0.2103639728562615</v>
       </c>
       <c r="C26" s="5">
-        <v>0.3875</v>
+        <v>0.375</v>
       </c>
       <c r="D26" s="5">
-        <v>0.8375</v>
+        <v>0.6</v>
       </c>
       <c r="E26" s="4">
-        <v>1.1</v>
+        <v>1.15</v>
       </c>
       <c r="F26" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:6">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="4">
-        <v>-0.0246856078248721</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>0.2081911262798635</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -1357,23 +715,23 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="5">
-        <v>0.8375</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="4">
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>0.925</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +739,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -1411,48 +769,48 @@
         <v>14</v>
       </c>
       <c r="B39" s="4">
-        <v>-0.0246856078248721</v>
+        <v>0.2081911262798635</v>
       </c>
       <c r="C39" s="5">
         <v>0.375</v>
       </c>
       <c r="D39" s="5">
-        <v>0.8375</v>
+        <v>0.625</v>
       </c>
       <c r="E39" s="4">
-        <v>0.8125</v>
+        <v>0.925</v>
       </c>
       <c r="F39" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="4">
-        <v>-0.0583941605839418</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>0.2717584369449378</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B45" s="5">
-        <v>0.425</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
         <v>5</v>
       </c>
@@ -1460,15 +818,15 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B47" s="4">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>0.6375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -1476,7 +834,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
         <v>8</v>
       </c>
@@ -1506,64 +864,64 @@
         <v>18</v>
       </c>
       <c r="B52" s="4">
-        <v>-0.0583941605839418</v>
+        <v>0.2717584369449378</v>
       </c>
       <c r="C52" s="5">
-        <v>0.425</v>
+        <v>0.55</v>
       </c>
       <c r="D52" s="5">
         <v>0.85</v>
       </c>
       <c r="E52" s="4">
-        <v>1.05</v>
+        <v>0.6375</v>
       </c>
       <c r="F52" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:6">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:6">
       <c r="A57" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B57" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>0.2061281337047354</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B58" s="5">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="5">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>0.725</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B60" s="4">
-        <v>1.125</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
@@ -1571,7 +929,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
         <v>8</v>
       </c>
@@ -1601,48 +959,48 @@
         <v>18</v>
       </c>
       <c r="B65" s="4">
-        <v>0</v>
+        <v>0.2061281337047354</v>
       </c>
       <c r="C65" s="5">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="D65" s="5">
-        <v>0.85</v>
+        <v>0.725</v>
       </c>
       <c r="E65" s="4">
-        <v>1.125</v>
+        <v>0.9375</v>
       </c>
       <c r="F65" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:6">
       <c r="A69" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:6">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="4">
-        <v>0.0287769784172661</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>0.3877551020408163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B71" s="5">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>0.5375</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="3" t="s">
         <v>5</v>
       </c>
@@ -1650,15 +1008,15 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:6">
       <c r="A73" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B73" s="4">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>0.5375</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="3" t="s">
         <v>7</v>
       </c>
@@ -1666,7 +1024,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
         <v>8</v>
       </c>
@@ -1696,48 +1054,48 @@
         <v>18</v>
       </c>
       <c r="B78" s="4">
-        <v>0.0287769784172661</v>
+        <v>0.3877551020408163</v>
       </c>
       <c r="C78" s="5">
-        <v>0.45</v>
+        <v>0.5375</v>
       </c>
       <c r="D78" s="5">
         <v>0.85</v>
       </c>
       <c r="E78" s="4">
-        <v>0.95</v>
+        <v>0.5375</v>
       </c>
       <c r="F78" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:6">
       <c r="A82" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:6">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B83" s="4">
-        <v>0.107736117702895</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>0.3973634651600754</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B84" s="5">
-        <v>0.475</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="3" t="s">
         <v>5</v>
       </c>
@@ -1745,15 +1103,15 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:6">
       <c r="A86" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B86" s="4">
-        <v>0.7375</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="3" t="s">
         <v>7</v>
       </c>
@@ -1761,7 +1119,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:6">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
@@ -1791,64 +1149,64 @@
         <v>22</v>
       </c>
       <c r="B91" s="4">
-        <v>0.107736117702895</v>
+        <v>0.3973634651600754</v>
       </c>
       <c r="C91" s="5">
-        <v>0.475</v>
+        <v>0.625</v>
       </c>
       <c r="D91" s="5">
         <v>0.85</v>
       </c>
       <c r="E91" s="4">
-        <v>0.7375</v>
+        <v>0.45</v>
       </c>
       <c r="F91" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:6">
       <c r="A94" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:6">
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:6">
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B96" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>0.1137664924072692</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B97" s="5">
-        <v>0.5125</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B98" s="5">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B99" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>1.7625</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="3" t="s">
         <v>7</v>
       </c>
@@ -1856,7 +1214,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:6">
       <c r="A102" s="2" t="s">
         <v>8</v>
       </c>
@@ -1886,64 +1244,64 @@
         <v>22</v>
       </c>
       <c r="B104" s="4">
-        <v>0</v>
+        <v>0.1137664924072692</v>
       </c>
       <c r="C104" s="5">
-        <v>0.5125</v>
+        <v>0.2</v>
       </c>
       <c r="D104" s="5">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="E104" s="4">
-        <v>1</v>
+        <v>1.7625</v>
       </c>
       <c r="F104" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:6">
       <c r="A107" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:6">
       <c r="A108" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:6">
       <c r="A109" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B109" s="4">
-        <v>0.110269758637009</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+        <v>0.2633279483037156</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B110" s="5">
-        <v>0.475</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
+        <v>0.4125</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B111" s="5">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B112" s="4">
-        <v>0.7375</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
+        <v>0.9625</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" s="3" t="s">
         <v>7</v>
       </c>
@@ -1951,7 +1309,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:6">
       <c r="A115" s="2" t="s">
         <v>8</v>
       </c>
@@ -1981,64 +1339,64 @@
         <v>22</v>
       </c>
       <c r="B117" s="4">
-        <v>0.110269758637009</v>
+        <v>0.2633279483037156</v>
       </c>
       <c r="C117" s="5">
-        <v>0.475</v>
+        <v>0.4125</v>
       </c>
       <c r="D117" s="5">
-        <v>0.85</v>
+        <v>0.625</v>
       </c>
       <c r="E117" s="4">
-        <v>0.7375</v>
+        <v>0.9625</v>
       </c>
       <c r="F117" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:6">
       <c r="A120" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:6">
       <c r="A121" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:6">
       <c r="A122" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B122" s="4">
-        <v>-0.051212938005391</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
+        <v>0.05000000000000004</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B123" s="5">
-        <v>0.525</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+        <v>0.2875</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B124" s="5">
-        <v>0.975</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B125" s="4">
-        <v>0.5125</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+        <v>0.7125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" s="3" t="s">
         <v>7</v>
       </c>
@@ -2046,7 +1404,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:6">
       <c r="A128" s="2" t="s">
         <v>8</v>
       </c>
@@ -2076,64 +1434,64 @@
         <v>26</v>
       </c>
       <c r="B130" s="4">
-        <v>-0.051212938005391</v>
+        <v>0.05000000000000004</v>
       </c>
       <c r="C130" s="5">
-        <v>0.525</v>
+        <v>0.2875</v>
       </c>
       <c r="D130" s="5">
-        <v>0.975</v>
+        <v>0.95</v>
       </c>
       <c r="E130" s="4">
-        <v>0.5125</v>
+        <v>0.7125</v>
       </c>
       <c r="F130" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:6">
       <c r="A133" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:6">
       <c r="A134" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:6">
       <c r="A135" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B135" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
+        <v>0.02540608079966689</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B136" s="5">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
+        <v>0.08749999999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B137" s="5">
-        <v>0.975</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
+        <v>0.4125</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B138" s="4">
-        <v>0.225</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
+        <v>2.6125</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" s="3" t="s">
         <v>7</v>
       </c>
@@ -2141,7 +1499,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:6">
       <c r="A141" s="2" t="s">
         <v>8</v>
       </c>
@@ -2171,64 +1529,64 @@
         <v>26</v>
       </c>
       <c r="B143" s="4">
-        <v>0</v>
+        <v>0.02540608079966689</v>
       </c>
       <c r="C143" s="5">
-        <v>0.85</v>
+        <v>0.08749999999999999</v>
       </c>
       <c r="D143" s="5">
-        <v>0.975</v>
+        <v>0.4125</v>
       </c>
       <c r="E143" s="4">
-        <v>0.225</v>
+        <v>2.6125</v>
       </c>
       <c r="F143" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:6">
       <c r="A147" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:6">
       <c r="A148" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B148" s="4">
-        <v>-0.0714285714285714</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
+        <v>0.03991370010787476</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B149" s="5">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B150" s="5">
-        <v>0.975</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B151" s="4">
-        <v>0.475</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
+        <v>1.7375</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" s="3" t="s">
         <v>7</v>
       </c>
@@ -2236,7 +1594,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:6">
       <c r="A154" s="2" t="s">
         <v>8</v>
       </c>
@@ -2266,16 +1624,16 @@
         <v>26</v>
       </c>
       <c r="B156" s="4">
-        <v>-0.0714285714285714</v>
+        <v>0.03991370010787476</v>
       </c>
       <c r="C156" s="5">
-        <v>0.5625</v>
+        <v>0.2</v>
       </c>
       <c r="D156" s="5">
-        <v>0.975</v>
+        <v>0.625</v>
       </c>
       <c r="E156" s="4">
-        <v>0.475</v>
+        <v>1.7375</v>
       </c>
       <c r="F156" s="3">
         <v>80</v>
@@ -2283,6 +1641,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>